<commit_message>
[opt] 优化excel中填写bool类型数据，可以用 true|yes|y|1表示true,用 false|no|n|0表示false
</commit_message>
<xml_diff>
--- a/MiniTemplate/Datas/item.xlsx
+++ b/MiniTemplate/Datas/item.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20328" windowHeight="9047"/>
+    <workbookView windowWidth="20304" windowHeight="8364"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="85">
   <si>
     <t>##var</t>
   </si>
@@ -254,6 +254,9 @@
     <t>初始下装</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>10004,3</t>
   </si>
   <si>
@@ -266,6 +269,9 @@
     <t>初始袜子</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>10005,4</t>
   </si>
   <si>
@@ -278,6 +284,9 @@
     <t>初始鞋子</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>PURPLE</t>
   </si>
   <si>
@@ -291,6 +300,9 @@
   </si>
   <si>
     <t>初始发饰</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
   <si>
     <t>10007,5</t>
@@ -345,7 +357,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,20 +375,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -868,10 +866,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -880,7 +878,7 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -889,134 +887,134 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="31" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="31" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="7" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="31" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1037,13 +1035,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1369,7 +1360,7 @@
   <dimension ref="A1:AI15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -1578,8 +1569,8 @@
       <c r="K4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="14"/>
-      <c r="M4" s="15"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="13"/>
       <c r="N4" s="9"/>
       <c r="O4"/>
       <c r="P4"/>
@@ -1684,19 +1675,19 @@
       <c r="H6" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="5" t="s">
         <v>40</v>
       </c>
       <c r="J6" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="16" t="s">
+      <c r="K6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="14">
         <v>10001</v>
       </c>
-      <c r="M6" s="17">
+      <c r="M6" s="14">
         <v>2</v>
       </c>
     </row>
@@ -1719,22 +1710,22 @@
       <c r="G7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H7" t="b">
+      <c r="H7">
         <v>0</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="5" t="s">
         <v>40</v>
       </c>
       <c r="J7" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="K7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7" s="14">
         <v>10001</v>
       </c>
-      <c r="M7" s="17">
+      <c r="M7" s="14">
         <v>3</v>
       </c>
     </row>
@@ -1757,22 +1748,22 @@
       <c r="G8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="16" t="s">
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>49</v>
       </c>
       <c r="J8" t="s">
         <v>50</v>
       </c>
-      <c r="K8" s="16" t="s">
+      <c r="K8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="14">
         <v>10001</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="14">
         <v>4</v>
       </c>
     </row>
@@ -1795,22 +1786,22 @@
       <c r="G9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="16" t="s">
+      <c r="H9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>49</v>
       </c>
       <c r="J9" t="s">
-        <v>54</v>
-      </c>
-      <c r="K9" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="L9" s="17">
+      <c r="K9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L9" s="14">
         <v>10001</v>
       </c>
-      <c r="M9" s="17">
+      <c r="M9" s="14">
         <v>5</v>
       </c>
     </row>
@@ -1819,10 +1810,10 @@
         <v>10004</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E10">
         <v>100</v>
@@ -1833,22 +1824,22 @@
       <c r="G10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="16" t="s">
+      <c r="H10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>49</v>
       </c>
       <c r="J10" t="s">
-        <v>58</v>
-      </c>
-      <c r="K10" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="L10" s="17">
+        <v>60</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10" s="14">
         <v>10001</v>
       </c>
-      <c r="M10" s="17">
+      <c r="M10" s="14">
         <v>6</v>
       </c>
     </row>
@@ -1857,10 +1848,10 @@
         <v>10005</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E11">
         <v>100</v>
@@ -1871,22 +1862,22 @@
       <c r="G11" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H11" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>62</v>
+      <c r="H11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="J11" t="s">
-        <v>63</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="L11" s="17">
+        <v>66</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" s="14">
         <v>10001</v>
       </c>
-      <c r="M11" s="17">
+      <c r="M11" s="14">
         <v>7</v>
       </c>
     </row>
@@ -1895,10 +1886,10 @@
         <v>10006</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E12">
         <v>100</v>
@@ -1909,22 +1900,22 @@
       <c r="G12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>62</v>
+      <c r="H12" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="J12" t="s">
-        <v>67</v>
-      </c>
-      <c r="K12" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="L12" s="17">
+        <v>71</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="L12" s="14">
         <v>10001</v>
       </c>
-      <c r="M12" s="17">
+      <c r="M12" s="14">
         <v>8</v>
       </c>
     </row>
@@ -1933,10 +1924,10 @@
         <v>10007</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E13">
         <v>200</v>
@@ -1950,19 +1941,19 @@
       <c r="H13" t="b">
         <v>0</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I13" s="5" t="s">
         <v>49</v>
       </c>
       <c r="J13" t="s">
-        <v>70</v>
-      </c>
-      <c r="K13" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="L13" s="17">
+        <v>74</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="L13" s="14">
         <v>10001</v>
       </c>
-      <c r="M13" s="17">
+      <c r="M13" s="14">
         <v>9</v>
       </c>
     </row>
@@ -1971,10 +1962,10 @@
         <v>10008</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E14">
         <v>300</v>
@@ -1988,19 +1979,19 @@
       <c r="H14" t="b">
         <v>0</v>
       </c>
-      <c r="I14" s="16" t="s">
-        <v>62</v>
+      <c r="I14" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="J14" t="s">
-        <v>73</v>
-      </c>
-      <c r="K14" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="L14" s="17">
+        <v>77</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="L14" s="14">
         <v>10001</v>
       </c>
-      <c r="M14" s="17">
+      <c r="M14" s="14">
         <v>10</v>
       </c>
     </row>
@@ -2009,10 +2000,10 @@
         <v>10009</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E15">
         <v>100</v>
@@ -2021,24 +2012,24 @@
         <v>10000</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="H15" t="b">
         <v>1</v>
       </c>
-      <c r="I15" s="16" t="s">
-        <v>78</v>
+      <c r="I15" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="J15" t="s">
-        <v>79</v>
-      </c>
-      <c r="K15" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="L15" s="17">
+        <v>83</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="L15" s="14">
         <v>10001</v>
       </c>
-      <c r="M15" s="17">
+      <c r="M15" s="14">
         <v>11</v>
       </c>
     </row>

</xml_diff>